<commit_message>
dashbord,addstudents,issuebook done and change in side nav also
</commit_message>
<xml_diff>
--- a/public/Students-list/6690f35c1f909326d1451ed8/student_data.xlsx
+++ b/public/Students-list/6690f35c1f909326d1451ed8/student_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20475" windowHeight="8220"/>
+    <workbookView windowWidth="20490" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1287,12 +1287,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="9.57142857142857" customWidth="1"/>
+    <col min="1" max="1" width="10.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="14.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>20220560</v>
+        <v>2022056840</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>20220561</v>
+        <v>2022056141</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>20220562</v>
+        <v>2022056142</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>20220563</v>
+        <v>2022056143</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>202205604</v>
+        <v>2022056014</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Issue book api changes done whine book issue qty decrement
</commit_message>
<xml_diff>
--- a/public/Students-list/6690f35c1f909326d1451ed8/student_data.xlsx
+++ b/public/Students-list/6690f35c1f909326d1451ed8/student_data.xlsx
@@ -56,10 +56,28 @@
     <t>studentDiv</t>
   </si>
   <si>
-    <t>E20229898984</t>
-  </si>
-  <si>
-    <t>suresh</t>
+    <t>E22110469000110028</t>
+  </si>
+  <si>
+    <t>vraj dalal</t>
+  </si>
+  <si>
+    <t>vrajdalal492@gmail.com</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>Third Year</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E22110469000110029</t>
+  </si>
+  <si>
+    <t>mukesh</t>
   </si>
   <si>
     <t>suresh@gmail.com</t>
@@ -68,61 +86,43 @@
     <t>BBA</t>
   </si>
   <si>
+    <t>First Year</t>
+  </si>
+  <si>
+    <t>E22110469000110030</t>
+  </si>
+  <si>
+    <t>ramesh</t>
+  </si>
+  <si>
+    <t>ramesh@gmail.com</t>
+  </si>
+  <si>
+    <t>BCOM</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E22110469000110031</t>
+  </si>
+  <si>
+    <t>nilesh</t>
+  </si>
+  <si>
+    <t>vrajdalal650@gmail.com</t>
+  </si>
+  <si>
     <t>Second Year</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>E20229898985</t>
-  </si>
-  <si>
-    <t>mukesh</t>
-  </si>
-  <si>
-    <t>vrajdalal492@gmail.com</t>
-  </si>
-  <si>
-    <t>BCA</t>
-  </si>
-  <si>
-    <t>First Year</t>
-  </si>
-  <si>
-    <t>E202298989846</t>
-  </si>
-  <si>
-    <t>ramesh</t>
-  </si>
-  <si>
-    <t>ramesh@gmail.com</t>
-  </si>
-  <si>
-    <t>BCOM</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>E20229898987</t>
-  </si>
-  <si>
-    <t>nilesh</t>
-  </si>
-  <si>
-    <t>vrajdalal650@gmail.com</t>
-  </si>
-  <si>
-    <t>E20229898988</t>
+    <t>E22110469000110032</t>
   </si>
   <si>
     <t>rajesh</t>
   </si>
   <si>
     <t>rajesh@gmail.com</t>
-  </si>
-  <si>
-    <t>Third Year</t>
   </si>
   <si>
     <t>C</t>
@@ -149,15 +149,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,10 +611,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -745,10 +745,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,16 +1287,16 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="10.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="14.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="20.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="19.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="24.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="18.1428571428571" customWidth="1"/>
     <col min="7" max="7" width="15.1428571428571" customWidth="1"/>
     <col min="8" max="8" width="12.5714285714286" customWidth="1"/>
@@ -1374,7 +1374,7 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F3">
@@ -1403,7 +1403,7 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4">
@@ -1432,17 +1432,17 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F5">
         <v>8978978988</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
@@ -1453,25 +1453,25 @@
         <v>2022056014</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F6">
         <v>8978978999</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
@@ -1479,11 +1479,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="suresh@gmail.com" tooltip="mailto:suresh@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="vrajdalal492@gmail.com" tooltip="mailto:vrajdalal492@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId3" display="ramesh@gmail.com" tooltip="mailto:ramesh@gmail.com"/>
-    <hyperlink ref="E5" r:id="rId4" display="vrajdalal650@gmail.com" tooltip="mailto:vrajdalal650@gmail.com"/>
-    <hyperlink ref="E6" r:id="rId5" display="rajesh@gmail.com" tooltip="mailto:rajesh@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId1" display="suresh@gmail.com" tooltip="mailto:suresh@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId2" display="ramesh@gmail.com" tooltip="mailto:ramesh@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId3" display="vrajdalal650@gmail.com" tooltip="mailto:vrajdalal650@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId4" display="rajesh@gmail.com" tooltip="mailto:rajesh@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId5" display="vrajdalal492@gmail.com" tooltip="mailto:vrajdalal492@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>